<commit_message>
adjusting for more buffs, and creating accurate and current printing document
</commit_message>
<xml_diff>
--- a/tactile_tabletop/Augment Cards/Tactile_Tabletop_Data-Augments.xlsx
+++ b/tactile_tabletop/Augment Cards/Tactile_Tabletop_Data-Augments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\TableTopRolePlaying_Squib\tactile_tabletop\Augment Cards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{618C0C0D-3A09-489D-AF7C-6EEBEB4C3A07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C556946-D655-4AFC-8E37-C346B5F1F6B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="149">
   <si>
     <t>Lunging Strike</t>
   </si>
@@ -398,9 +398,6 @@
     <t>gain 5ft of movement each turn in combat. Any time you spend 6 seconds (one round) without moving, your next roll is -3</t>
   </si>
   <si>
-    <t>Wait a week</t>
-  </si>
-  <si>
     <t>The end is never the end is never the end</t>
   </si>
   <si>
@@ -413,9 +410,6 @@
     <t>When your current health is within 25% of max, reduce attack values by 2. when your current health is within 25% of min, instead increase attack values by 2</t>
   </si>
   <si>
-    <t>Roll a 3 four times</t>
-  </si>
-  <si>
     <t>The stars aren't happy with you</t>
   </si>
   <si>
@@ -437,19 +431,43 @@
     <t>20 ft movement - hand</t>
   </si>
   <si>
-    <t>Become downed three times</t>
-  </si>
-  <si>
-    <t>Heal 50 points worth of health from rest</t>
-  </si>
-  <si>
-    <t>Drink a gallon of blood</t>
-  </si>
-  <si>
-    <t>Spirit Boon</t>
-  </si>
-  <si>
-    <t>A spectre floats just behind you at all times. Choose 1 buff: +1 all influence, +1 all defence, +1 all attack</t>
+    <t>Eyes of the fallen</t>
+  </si>
+  <si>
+    <t>Flames of ambition</t>
+  </si>
+  <si>
+    <t>Half of your body is scarred. Gain +2 to influence values when within 15 ft of an open flame</t>
+  </si>
+  <si>
+    <t>Spectre of Death</t>
+  </si>
+  <si>
+    <t>Beastial Mark</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your eyes are blackened completely. You gain +4 to any roll that involves percieving </t>
+  </si>
+  <si>
+    <t>Small horns grow from the top of your head, and your body hair grows thicker. Defense values are increased by 2</t>
+  </si>
+  <si>
+    <t>A mostly transparent spectre floats just behind you at all times, about an inch behind and above you. At the start of each turn, choose to increase your influence, defense, or attack by 1</t>
+  </si>
+  <si>
+    <t>Roll a 3 four times, then card transforms</t>
+  </si>
+  <si>
+    <t>Wait a week, then card transforms</t>
+  </si>
+  <si>
+    <t>Drink a gallon of blood, then card transforms</t>
+  </si>
+  <si>
+    <t>Heal 50 points worth of health from rest, then card transforms</t>
+  </si>
+  <si>
+    <t>Become downed three times, then card transforms</t>
   </si>
 </sst>
 </file>
@@ -939,11 +957,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1304,148 +1319,178 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.28515625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="25.5703125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" style="4" customWidth="1"/>
-    <col min="6" max="6" width="38.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8" style="4" customWidth="1"/>
-    <col min="8" max="8" width="34.85546875" style="4" customWidth="1"/>
-    <col min="9" max="9" width="30.28515625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="30.42578125" style="4" customWidth="1"/>
-    <col min="11" max="11" width="21.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.140625" style="4" customWidth="1"/>
-    <col min="13" max="13" width="7.85546875" style="4" customWidth="1"/>
-    <col min="14" max="14" width="13.85546875" style="4" customWidth="1"/>
-    <col min="15" max="15" width="18.28515625" style="4" customWidth="1"/>
-    <col min="16" max="16" width="45.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.42578125" style="4" customWidth="1"/>
-    <col min="18" max="18" width="11.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.7109375" style="4" customWidth="1"/>
-    <col min="20" max="20" width="33.140625" style="4" customWidth="1"/>
-    <col min="21" max="21" width="44.42578125" style="4" customWidth="1"/>
-    <col min="22" max="22" width="43.42578125" style="4" customWidth="1"/>
-    <col min="23" max="16384" width="22.28515625" style="4"/>
+    <col min="1" max="1" width="20.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.28515625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="25.5703125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="38.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8" style="3" customWidth="1"/>
+    <col min="8" max="8" width="34.85546875" style="3" customWidth="1"/>
+    <col min="9" max="9" width="30.28515625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="30.42578125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="21.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.140625" style="3" customWidth="1"/>
+    <col min="13" max="13" width="7.85546875" style="3" customWidth="1"/>
+    <col min="14" max="14" width="13.85546875" style="3" customWidth="1"/>
+    <col min="15" max="15" width="18.28515625" style="3" customWidth="1"/>
+    <col min="16" max="16" width="45.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.42578125" style="3" customWidth="1"/>
+    <col min="18" max="18" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.7109375" style="3" customWidth="1"/>
+    <col min="20" max="20" width="33.140625" style="3" customWidth="1"/>
+    <col min="21" max="21" width="44.42578125" style="3" customWidth="1"/>
+    <col min="22" max="22" width="43.42578125" style="3" customWidth="1"/>
+    <col min="23" max="16384" width="22.28515625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="D6" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="B3" s="4" t="s">
+      <c r="B9" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="90" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="D4" s="4" t="s">
+      <c r="B10" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="C8" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C19" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
@@ -1668,7 +1713,7 @@
       <c r="A23" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C23" t="s">
@@ -1789,7 +1834,7 @@
       <c r="A37" t="s">
         <v>63</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="2" t="s">
         <v>64</v>
       </c>
       <c r="C37" t="s">
@@ -1811,13 +1856,13 @@
       <c r="A39" t="s">
         <v>51</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C39" t="s">
         <v>34</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D39" s="1" t="s">
         <v>107</v>
       </c>
     </row>
@@ -1825,7 +1870,7 @@
       <c r="A40" t="s">
         <v>35</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="1" t="s">
         <v>36</v>
       </c>
       <c r="C40" t="s">

</xml_diff>

<commit_message>
excel sheet updates aligning to character card data
</commit_message>
<xml_diff>
--- a/tactile_tabletop/Augment Cards/Tactile_Tabletop_Data-Augments.xlsx
+++ b/tactile_tabletop/Augment Cards/Tactile_Tabletop_Data-Augments.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\TableTopRolePlaying_Squib\tactile_tabletop\Augment Cards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C556946-D655-4AFC-8E37-C346B5F1F6B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06903551-99C9-481B-9AF4-CE06AC6A880D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,12 +16,24 @@
     <sheet name="Tactile Tabletop Data - Level 1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="173">
   <si>
     <t>Lunging Strike</t>
   </si>
@@ -377,27 +389,12 @@
     <t>must get attacked in round following attack, must defend against all damage, discard</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Variables</t>
-  </si>
-  <si>
-    <t>Rules</t>
-  </si>
-  <si>
-    <t>Conditions to Remove</t>
-  </si>
-  <si>
     <t>Roll a 1d3. On a 1, reduce each calculated attack value by 1 for the rest of the day. On a 2, it's to defense.</t>
   </si>
   <si>
     <t>You should run</t>
   </si>
   <si>
-    <t>gain 5ft of movement each turn in combat. Any time you spend 6 seconds (one round) without moving, your next roll is -3</t>
-  </si>
-  <si>
     <t>The end is never the end is never the end</t>
   </si>
   <si>
@@ -425,12 +422,6 @@
     <t>Your limbs are permanently stained black, as though thrust into a pot of ink. During the night, any movement you take is increased by 5 ft, and all attack values gain +1</t>
   </si>
   <si>
-    <t>Attack - discard</t>
-  </si>
-  <si>
-    <t>20 ft movement - hand</t>
-  </si>
-  <si>
     <t>Eyes of the fallen</t>
   </si>
   <si>
@@ -468,6 +459,99 @@
   </si>
   <si>
     <t>Become downed three times, then card transforms</t>
+  </si>
+  <si>
+    <t>Tier</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Top Ability Name</t>
+  </si>
+  <si>
+    <t>Top Ability Target</t>
+  </si>
+  <si>
+    <t>Top Ability Duration</t>
+  </si>
+  <si>
+    <t>Top Ability Die Roll/Scaler</t>
+  </si>
+  <si>
+    <t>Top Weapon Or Influence</t>
+  </si>
+  <si>
+    <t>Top Ability Rules</t>
+  </si>
+  <si>
+    <t>Top Ability Following Card Action</t>
+  </si>
+  <si>
+    <t>Bottom Ability Name</t>
+  </si>
+  <si>
+    <t>Bottom Ability Target</t>
+  </si>
+  <si>
+    <t>Bottom Ability Duration</t>
+  </si>
+  <si>
+    <t>Bottom Ability Die Roll/Scaler</t>
+  </si>
+  <si>
+    <t>Bottom Weapon Or Influence</t>
+  </si>
+  <si>
+    <t>Bottom Ability Rules</t>
+  </si>
+  <si>
+    <t>Bottom Ability Following Card Action</t>
+  </si>
+  <si>
+    <t>Requirements</t>
+  </si>
+  <si>
+    <t>Instant</t>
+  </si>
+  <si>
+    <t>Weapon</t>
+  </si>
+  <si>
+    <t>Discard</t>
+  </si>
+  <si>
+    <t>Enemy</t>
+  </si>
+  <si>
+    <t>Attack!</t>
+  </si>
+  <si>
+    <t>Attack</t>
+  </si>
+  <si>
+    <t>Passive Name</t>
+  </si>
+  <si>
+    <t>Start each round with 5 ft movement. Any time you spend 6 seconds (one round) without moving, your next roll is -3</t>
+  </si>
+  <si>
+    <t>Run!</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Gain 20 additional feet of movement</t>
+  </si>
+  <si>
+    <t>Hand</t>
+  </si>
+  <si>
+    <t>Passive Rules</t>
+  </si>
+  <si>
+    <t>none. This is a good thing. Why, you want to get rid of a good thing?</t>
   </si>
 </sst>
 </file>
@@ -957,11 +1041,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1319,11 +1406,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:X11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1334,163 +1421,727 @@
     <col min="4" max="4" width="25.5703125" style="3" customWidth="1"/>
     <col min="5" max="5" width="14.85546875" style="3" customWidth="1"/>
     <col min="6" max="6" width="38.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8" style="3" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" style="3" customWidth="1"/>
     <col min="8" max="8" width="34.85546875" style="3" customWidth="1"/>
     <col min="9" max="9" width="30.28515625" style="3" customWidth="1"/>
     <col min="10" max="10" width="30.42578125" style="3" customWidth="1"/>
     <col min="11" max="11" width="21.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="20.140625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="7.85546875" style="3" customWidth="1"/>
-    <col min="14" max="14" width="13.85546875" style="3" customWidth="1"/>
+    <col min="13" max="14" width="17" style="3" customWidth="1"/>
     <col min="15" max="15" width="18.28515625" style="3" customWidth="1"/>
     <col min="16" max="16" width="45.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.42578125" style="3" customWidth="1"/>
-    <col min="18" max="18" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.7109375" style="3" customWidth="1"/>
-    <col min="20" max="20" width="33.140625" style="3" customWidth="1"/>
-    <col min="21" max="21" width="44.42578125" style="3" customWidth="1"/>
-    <col min="22" max="22" width="43.42578125" style="3" customWidth="1"/>
-    <col min="23" max="16384" width="22.28515625" style="3"/>
+    <col min="17" max="18" width="30.85546875" style="3" customWidth="1"/>
+    <col min="19" max="19" width="15.28515625" style="3" customWidth="1"/>
+    <col min="20" max="20" width="13.7109375" style="3" customWidth="1"/>
+    <col min="21" max="21" width="33.140625" style="3" customWidth="1"/>
+    <col min="22" max="22" width="44.42578125" style="3" customWidth="1"/>
+    <col min="23" max="23" width="43.42578125" style="3" customWidth="1"/>
+    <col min="24" max="16384" width="22.28515625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H1" t="s">
+        <v>149</v>
+      </c>
+      <c r="I1" t="s">
+        <v>150</v>
+      </c>
+      <c r="J1" t="s">
+        <v>151</v>
+      </c>
+      <c r="K1" t="s">
+        <v>152</v>
+      </c>
+      <c r="L1" t="s">
+        <v>153</v>
+      </c>
+      <c r="M1" t="s">
+        <v>154</v>
+      </c>
+      <c r="N1" t="s">
+        <v>155</v>
+      </c>
+      <c r="O1" t="s">
+        <v>156</v>
+      </c>
+      <c r="P1" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>165</v>
+      </c>
+      <c r="R1" t="s">
+        <v>171</v>
+      </c>
+      <c r="S1" t="s">
+        <v>158</v>
+      </c>
+      <c r="T1"/>
+      <c r="U1"/>
+      <c r="V1"/>
+      <c r="W1"/>
+      <c r="X1"/>
+    </row>
+    <row r="2" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E2" t="s">
+        <v>159</v>
+      </c>
+      <c r="F2" t="s">
+        <v>164</v>
+      </c>
+      <c r="G2" t="s">
+        <v>160</v>
+      </c>
+      <c r="H2" t="s">
+        <v>168</v>
+      </c>
+      <c r="I2" t="s">
+        <v>161</v>
+      </c>
+      <c r="J2" t="s">
+        <v>163</v>
+      </c>
+      <c r="K2" t="s">
+        <v>162</v>
+      </c>
+      <c r="L2" t="s">
+        <v>159</v>
+      </c>
+      <c r="M2" t="s">
+        <v>164</v>
+      </c>
+      <c r="N2" t="s">
+        <v>160</v>
+      </c>
+      <c r="O2" t="s">
+        <v>168</v>
+      </c>
+      <c r="P2" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>124</v>
+      </c>
+      <c r="R2" t="s">
         <v>118</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="S2" t="s">
+        <v>137</v>
+      </c>
+      <c r="T2"/>
+      <c r="U2"/>
+      <c r="V2"/>
+      <c r="W2"/>
+      <c r="X2"/>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>167</v>
+      </c>
+      <c r="D3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E3" t="s">
+        <v>168</v>
+      </c>
+      <c r="F3" t="s">
+        <v>168</v>
+      </c>
+      <c r="G3" t="s">
+        <v>168</v>
+      </c>
+      <c r="H3" t="s">
+        <v>169</v>
+      </c>
+      <c r="I3" t="s">
+        <v>170</v>
+      </c>
+      <c r="J3" t="s">
+        <v>167</v>
+      </c>
+      <c r="K3" t="s">
+        <v>168</v>
+      </c>
+      <c r="L3" t="s">
+        <v>168</v>
+      </c>
+      <c r="M3" t="s">
+        <v>168</v>
+      </c>
+      <c r="N3" t="s">
+        <v>168</v>
+      </c>
+      <c r="O3" t="s">
+        <v>169</v>
+      </c>
+      <c r="P3" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q3" t="s">
         <v>119</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="R3" t="s">
+        <v>166</v>
+      </c>
+      <c r="S3" t="s">
+        <v>138</v>
+      </c>
+      <c r="T3"/>
+      <c r="U3"/>
+      <c r="V3"/>
+      <c r="W3"/>
+      <c r="X3"/>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>163</v>
+      </c>
+      <c r="D4" t="s">
+        <v>162</v>
+      </c>
+      <c r="E4" t="s">
+        <v>159</v>
+      </c>
+      <c r="F4" t="s">
+        <v>164</v>
+      </c>
+      <c r="G4" t="s">
+        <v>160</v>
+      </c>
+      <c r="H4" t="s">
+        <v>168</v>
+      </c>
+      <c r="I4" t="s">
+        <v>161</v>
+      </c>
+      <c r="J4" t="s">
+        <v>163</v>
+      </c>
+      <c r="K4" t="s">
+        <v>162</v>
+      </c>
+      <c r="L4" t="s">
+        <v>159</v>
+      </c>
+      <c r="M4" t="s">
+        <v>164</v>
+      </c>
+      <c r="N4" t="s">
+        <v>160</v>
+      </c>
+      <c r="O4" t="s">
+        <v>168</v>
+      </c>
+      <c r="P4" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>122</v>
+      </c>
+      <c r="R4" t="s">
+        <v>121</v>
+      </c>
+      <c r="S4" t="s">
+        <v>139</v>
+      </c>
+      <c r="T4"/>
+      <c r="U4"/>
+      <c r="V4"/>
+      <c r="W4"/>
+      <c r="X4"/>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>163</v>
+      </c>
+      <c r="D5" t="s">
+        <v>162</v>
+      </c>
+      <c r="E5" t="s">
+        <v>159</v>
+      </c>
+      <c r="F5" t="s">
+        <v>164</v>
+      </c>
+      <c r="G5" t="s">
+        <v>160</v>
+      </c>
+      <c r="H5" t="s">
+        <v>168</v>
+      </c>
+      <c r="I5" t="s">
+        <v>161</v>
+      </c>
+      <c r="J5" t="s">
+        <v>163</v>
+      </c>
+      <c r="K5" t="s">
+        <v>162</v>
+      </c>
+      <c r="L5" t="s">
+        <v>159</v>
+      </c>
+      <c r="M5" t="s">
+        <v>164</v>
+      </c>
+      <c r="N5" t="s">
+        <v>160</v>
+      </c>
+      <c r="O5" t="s">
+        <v>168</v>
+      </c>
+      <c r="P5" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>125</v>
+      </c>
+      <c r="R5" t="s">
+        <v>123</v>
+      </c>
+      <c r="S5" t="s">
+        <v>140</v>
+      </c>
+      <c r="T5"/>
+      <c r="U5"/>
+      <c r="V5"/>
+      <c r="W5"/>
+      <c r="X5"/>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>163</v>
+      </c>
+      <c r="D6" t="s">
+        <v>162</v>
+      </c>
+      <c r="E6" t="s">
+        <v>159</v>
+      </c>
+      <c r="F6" t="s">
+        <v>164</v>
+      </c>
+      <c r="G6" t="s">
+        <v>160</v>
+      </c>
+      <c r="H6" t="s">
+        <v>168</v>
+      </c>
+      <c r="I6" t="s">
+        <v>161</v>
+      </c>
+      <c r="J6" t="s">
+        <v>163</v>
+      </c>
+      <c r="K6" t="s">
+        <v>162</v>
+      </c>
+      <c r="L6" t="s">
+        <v>159</v>
+      </c>
+      <c r="M6" t="s">
+        <v>164</v>
+      </c>
+      <c r="N6" t="s">
+        <v>160</v>
+      </c>
+      <c r="O6" t="s">
+        <v>168</v>
+      </c>
+      <c r="P6" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q6" t="s">
         <v>120</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="R6" t="s">
+        <v>126</v>
+      </c>
+      <c r="S6" t="s">
+        <v>141</v>
+      </c>
+      <c r="T6"/>
+      <c r="U6"/>
+      <c r="V6"/>
+      <c r="W6"/>
+      <c r="X6"/>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>163</v>
+      </c>
+      <c r="D7" t="s">
+        <v>162</v>
+      </c>
+      <c r="E7" t="s">
+        <v>159</v>
+      </c>
+      <c r="F7" t="s">
+        <v>164</v>
+      </c>
+      <c r="G7" t="s">
+        <v>160</v>
+      </c>
+      <c r="H7" t="s">
+        <v>168</v>
+      </c>
+      <c r="I7" t="s">
+        <v>161</v>
+      </c>
+      <c r="J7" t="s">
+        <v>163</v>
+      </c>
+      <c r="K7" t="s">
+        <v>162</v>
+      </c>
+      <c r="L7" t="s">
+        <v>159</v>
+      </c>
+      <c r="M7" t="s">
+        <v>164</v>
+      </c>
+      <c r="N7" t="s">
+        <v>160</v>
+      </c>
+      <c r="O7" t="s">
+        <v>168</v>
+      </c>
+      <c r="P7" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>127</v>
+      </c>
+      <c r="R7" t="s">
+        <v>128</v>
+      </c>
+      <c r="S7" t="s">
+        <v>172</v>
+      </c>
+      <c r="T7"/>
+      <c r="U7"/>
+      <c r="V7"/>
+      <c r="W7"/>
+      <c r="X7"/>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>163</v>
+      </c>
+      <c r="D8" t="s">
+        <v>162</v>
+      </c>
+      <c r="E8" t="s">
+        <v>159</v>
+      </c>
+      <c r="F8" t="s">
+        <v>164</v>
+      </c>
+      <c r="G8" t="s">
+        <v>160</v>
+      </c>
+      <c r="H8" t="s">
+        <v>168</v>
+      </c>
+      <c r="I8" t="s">
+        <v>161</v>
+      </c>
+      <c r="J8" t="s">
+        <v>163</v>
+      </c>
+      <c r="K8" t="s">
+        <v>162</v>
+      </c>
+      <c r="L8" t="s">
+        <v>159</v>
+      </c>
+      <c r="M8" t="s">
+        <v>164</v>
+      </c>
+      <c r="N8" t="s">
+        <v>160</v>
+      </c>
+      <c r="O8" t="s">
+        <v>168</v>
+      </c>
+      <c r="P8" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>132</v>
+      </c>
+      <c r="R8" t="s">
+        <v>136</v>
+      </c>
+      <c r="S8" t="s">
+        <v>172</v>
+      </c>
+      <c r="T8"/>
+      <c r="U8"/>
+      <c r="V8"/>
+      <c r="W8"/>
+      <c r="X8"/>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>163</v>
+      </c>
+      <c r="D9" t="s">
+        <v>162</v>
+      </c>
+      <c r="E9" t="s">
+        <v>159</v>
+      </c>
+      <c r="F9" t="s">
+        <v>164</v>
+      </c>
+      <c r="G9" t="s">
+        <v>160</v>
+      </c>
+      <c r="H9" t="s">
+        <v>168</v>
+      </c>
+      <c r="I9" t="s">
+        <v>161</v>
+      </c>
+      <c r="J9" t="s">
+        <v>163</v>
+      </c>
+      <c r="K9" t="s">
+        <v>162</v>
+      </c>
+      <c r="L9" t="s">
+        <v>159</v>
+      </c>
+      <c r="M9" t="s">
+        <v>164</v>
+      </c>
+      <c r="N9" t="s">
+        <v>160</v>
+      </c>
+      <c r="O9" t="s">
+        <v>168</v>
+      </c>
+      <c r="P9" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q9" t="s">
         <v>129</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="R9" t="s">
         <v>134</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="S9" t="s">
+        <v>172</v>
+      </c>
+      <c r="T9"/>
+      <c r="U9"/>
+      <c r="V9"/>
+      <c r="W9"/>
+      <c r="X9"/>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>163</v>
+      </c>
+      <c r="D10" t="s">
+        <v>162</v>
+      </c>
+      <c r="E10" t="s">
+        <v>159</v>
+      </c>
+      <c r="F10" t="s">
+        <v>164</v>
+      </c>
+      <c r="G10" t="s">
+        <v>160</v>
+      </c>
+      <c r="H10" t="s">
+        <v>168</v>
+      </c>
+      <c r="I10" t="s">
+        <v>161</v>
+      </c>
+      <c r="J10" t="s">
+        <v>163</v>
+      </c>
+      <c r="K10" t="s">
+        <v>162</v>
+      </c>
+      <c r="L10" t="s">
+        <v>159</v>
+      </c>
+      <c r="M10" t="s">
+        <v>164</v>
+      </c>
+      <c r="N10" t="s">
+        <v>160</v>
+      </c>
+      <c r="O10" t="s">
+        <v>168</v>
+      </c>
+      <c r="P10" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>130</v>
+      </c>
+      <c r="R10" t="s">
+        <v>131</v>
+      </c>
+      <c r="S10" t="s">
+        <v>172</v>
+      </c>
+      <c r="T10"/>
+      <c r="U10"/>
+      <c r="V10"/>
+      <c r="W10"/>
+      <c r="X10"/>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>163</v>
+      </c>
+      <c r="D11" t="s">
+        <v>162</v>
+      </c>
+      <c r="E11" t="s">
+        <v>159</v>
+      </c>
+      <c r="F11" t="s">
+        <v>164</v>
+      </c>
+      <c r="G11" t="s">
+        <v>160</v>
+      </c>
+      <c r="H11" t="s">
+        <v>168</v>
+      </c>
+      <c r="I11" t="s">
+        <v>161</v>
+      </c>
+      <c r="J11" t="s">
+        <v>163</v>
+      </c>
+      <c r="K11" t="s">
+        <v>162</v>
+      </c>
+      <c r="L11" t="s">
+        <v>159</v>
+      </c>
+      <c r="M11" t="s">
+        <v>164</v>
+      </c>
+      <c r="N11" t="s">
+        <v>160</v>
+      </c>
+      <c r="O11" t="s">
+        <v>168</v>
+      </c>
+      <c r="P11" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>133</v>
+      </c>
+      <c r="R11" t="s">
         <v>135</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="90" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="90" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>142</v>
-      </c>
+      <c r="S11" t="s">
+        <v>172</v>
+      </c>
+      <c r="T11"/>
+      <c r="U11"/>
+      <c r="V11"/>
+      <c r="W11"/>
+      <c r="X11"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>

<commit_message>
final tweaks to augment cards
</commit_message>
<xml_diff>
--- a/tactile_tabletop/Augment Cards/Tactile_Tabletop_Data-Augments.xlsx
+++ b/tactile_tabletop/Augment Cards/Tactile_Tabletop_Data-Augments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\TableTopRolePlaying_Squib\tactile_tabletop\Augment Cards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06903551-99C9-481B-9AF4-CE06AC6A880D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41CB6854-F70F-44A0-9026-3C6832700D99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tactile Tabletop Data - Level 1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="173">
   <si>
     <t>Lunging Strike</t>
   </si>
@@ -1410,7 +1410,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I17" sqref="I17"/>
+      <selection pane="bottomLeft" activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1525,9 +1525,7 @@
       <c r="G2" t="s">
         <v>160</v>
       </c>
-      <c r="H2" t="s">
-        <v>168</v>
-      </c>
+      <c r="H2"/>
       <c r="I2" t="s">
         <v>161</v>
       </c>
@@ -1546,9 +1544,7 @@
       <c r="N2" t="s">
         <v>160</v>
       </c>
-      <c r="O2" t="s">
-        <v>168</v>
-      </c>
+      <c r="O2"/>
       <c r="P2" t="s">
         <v>161</v>
       </c>
@@ -1584,14 +1580,11 @@
         <v>168</v>
       </c>
       <c r="F3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="G3" t="s">
         <v>168</v>
       </c>
-      <c r="H3" t="s">
-        <v>169</v>
-      </c>
       <c r="I3" t="s">
         <v>170</v>
       </c>
@@ -1605,13 +1598,10 @@
         <v>168</v>
       </c>
       <c r="M3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="N3" t="s">
         <v>168</v>
-      </c>
-      <c r="O3" t="s">
-        <v>169</v>
       </c>
       <c r="P3" t="s">
         <v>170</v>
@@ -1653,9 +1643,7 @@
       <c r="G4" t="s">
         <v>160</v>
       </c>
-      <c r="H4" t="s">
-        <v>168</v>
-      </c>
+      <c r="H4"/>
       <c r="I4" t="s">
         <v>161</v>
       </c>
@@ -1674,9 +1662,7 @@
       <c r="N4" t="s">
         <v>160</v>
       </c>
-      <c r="O4" t="s">
-        <v>168</v>
-      </c>
+      <c r="O4"/>
       <c r="P4" t="s">
         <v>161</v>
       </c>
@@ -1717,9 +1703,7 @@
       <c r="G5" t="s">
         <v>160</v>
       </c>
-      <c r="H5" t="s">
-        <v>168</v>
-      </c>
+      <c r="H5"/>
       <c r="I5" t="s">
         <v>161</v>
       </c>
@@ -1738,9 +1722,7 @@
       <c r="N5" t="s">
         <v>160</v>
       </c>
-      <c r="O5" t="s">
-        <v>168</v>
-      </c>
+      <c r="O5"/>
       <c r="P5" t="s">
         <v>161</v>
       </c>
@@ -1781,9 +1763,7 @@
       <c r="G6" t="s">
         <v>160</v>
       </c>
-      <c r="H6" t="s">
-        <v>168</v>
-      </c>
+      <c r="H6"/>
       <c r="I6" t="s">
         <v>161</v>
       </c>
@@ -1802,9 +1782,7 @@
       <c r="N6" t="s">
         <v>160</v>
       </c>
-      <c r="O6" t="s">
-        <v>168</v>
-      </c>
+      <c r="O6"/>
       <c r="P6" t="s">
         <v>161</v>
       </c>
@@ -1845,9 +1823,7 @@
       <c r="G7" t="s">
         <v>160</v>
       </c>
-      <c r="H7" t="s">
-        <v>168</v>
-      </c>
+      <c r="H7"/>
       <c r="I7" t="s">
         <v>161</v>
       </c>
@@ -1866,9 +1842,7 @@
       <c r="N7" t="s">
         <v>160</v>
       </c>
-      <c r="O7" t="s">
-        <v>168</v>
-      </c>
+      <c r="O7"/>
       <c r="P7" t="s">
         <v>161</v>
       </c>
@@ -1909,9 +1883,7 @@
       <c r="G8" t="s">
         <v>160</v>
       </c>
-      <c r="H8" t="s">
-        <v>168</v>
-      </c>
+      <c r="H8"/>
       <c r="I8" t="s">
         <v>161</v>
       </c>
@@ -1930,9 +1902,7 @@
       <c r="N8" t="s">
         <v>160</v>
       </c>
-      <c r="O8" t="s">
-        <v>168</v>
-      </c>
+      <c r="O8"/>
       <c r="P8" t="s">
         <v>161</v>
       </c>
@@ -1973,9 +1943,7 @@
       <c r="G9" t="s">
         <v>160</v>
       </c>
-      <c r="H9" t="s">
-        <v>168</v>
-      </c>
+      <c r="H9"/>
       <c r="I9" t="s">
         <v>161</v>
       </c>
@@ -1994,9 +1962,7 @@
       <c r="N9" t="s">
         <v>160</v>
       </c>
-      <c r="O9" t="s">
-        <v>168</v>
-      </c>
+      <c r="O9"/>
       <c r="P9" t="s">
         <v>161</v>
       </c>
@@ -2037,9 +2003,7 @@
       <c r="G10" t="s">
         <v>160</v>
       </c>
-      <c r="H10" t="s">
-        <v>168</v>
-      </c>
+      <c r="H10"/>
       <c r="I10" t="s">
         <v>161</v>
       </c>
@@ -2058,9 +2022,7 @@
       <c r="N10" t="s">
         <v>160</v>
       </c>
-      <c r="O10" t="s">
-        <v>168</v>
-      </c>
+      <c r="O10"/>
       <c r="P10" t="s">
         <v>161</v>
       </c>
@@ -2101,9 +2063,7 @@
       <c r="G11" t="s">
         <v>160</v>
       </c>
-      <c r="H11" t="s">
-        <v>168</v>
-      </c>
+      <c r="H11"/>
       <c r="I11" t="s">
         <v>161</v>
       </c>
@@ -2122,9 +2082,7 @@
       <c r="N11" t="s">
         <v>160</v>
       </c>
-      <c r="O11" t="s">
-        <v>168</v>
-      </c>
+      <c r="O11"/>
       <c r="P11" t="s">
         <v>161</v>
       </c>

</xml_diff>